<commit_message>
Apply revisions to economic feasibility
</commit_message>
<xml_diff>
--- a/docs/flux.xlsx
+++ b/docs/flux.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BGM\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BGM\Desktop\tesis\Thesis\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3114DB0B-163C-4A13-98C8-2B602ED574A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBEB917-7697-4BF8-9BAF-380ED5D7EAB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17205" yWindow="0" windowWidth="11595" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Desarrollo de Software</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Flujo</t>
   </si>
   <si>
-    <t>VAC</t>
-  </si>
-  <si>
     <t>1. TMAR</t>
   </si>
   <si>
@@ -102,32 +99,29 @@
     <t>Flujo Total</t>
   </si>
   <si>
-    <t>2. VAC (Desarrollo del Proyecto)</t>
-  </si>
-  <si>
-    <t>2. VAC (Mantenimiento del Proyecto)</t>
-  </si>
-  <si>
     <t>Mantenimiento de Software</t>
   </si>
   <si>
     <t>Inflación Promedio (anual)</t>
   </si>
   <si>
-    <t>Inflación Promedio (mensual)</t>
-  </si>
-  <si>
     <t>Inflación y Prima de Riesgo</t>
+  </si>
+  <si>
+    <t>VAN</t>
+  </si>
+  <si>
+    <t>2. VAN (Mantenimiento del Proyecto)</t>
+  </si>
+  <si>
+    <t>2. VAN (Desarrollo del Proyecto)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.00000"/>
-  </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +149,13 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -170,7 +171,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -240,29 +241,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -271,22 +255,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -566,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +562,7 @@
   <sheetData>
     <row r="2" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -591,32 +574,32 @@
     </row>
     <row r="3" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="5">
-        <f>N5+N6+(N5*N6)</f>
-        <v>0.21425265763166329</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="12"/>
+        <v>6</v>
+      </c>
+      <c r="E3" s="14">
+        <f>N4+N5+(N4*N5)</f>
+        <v>0.26202999999999999</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="8"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="16">
+      <c r="K4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="15">
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -625,23 +608,12 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-      <c r="K5" s="14" t="s">
-        <v>14</v>
+      <c r="K5" s="12" t="s">
+        <v>7</v>
       </c>
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
-      <c r="N5" s="15">
-        <f>((1+N4)^(1/12)) - 1</f>
-        <v>3.5145930840192463E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="17">
+      <c r="N5" s="16">
         <v>0.21</v>
       </c>
     </row>
@@ -749,7 +721,7 @@
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13">
         <f>SUM(D12:I12)</f>
@@ -757,55 +729,16 @@
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D14" s="5">
-        <f>(1+0.2143)^D7</f>
-        <v>1.2142999999999999</v>
-      </c>
-      <c r="E14" s="5">
-        <f t="shared" ref="E14:G14" si="0">(1+0.2143)^E7</f>
-        <v>1.4745244899999999</v>
-      </c>
-      <c r="F14" s="5">
-        <f t="shared" si="0"/>
-        <v>1.7905150882069998</v>
-      </c>
-      <c r="G14" s="5">
-        <f t="shared" si="0"/>
-        <v>2.1742224716097596</v>
-      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D15">
-        <f>D12/D14</f>
-        <v>462528.20555052295</v>
-      </c>
-      <c r="E15">
-        <f>E12/E14</f>
-        <v>380901.09985219716</v>
-      </c>
-      <c r="F15">
-        <f>F12/F14</f>
-        <v>313679.56835394644</v>
-      </c>
-      <c r="G15">
-        <f>G12/G14</f>
-        <v>258321.31133488138</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16">
-        <f>C15+(SUM(D15:I15))</f>
-        <v>1415430.1850915481</v>
-      </c>
-    </row>
     <row r="18" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -835,13 +768,11 @@
       <c r="H20" s="2">
         <v>5</v>
       </c>
-      <c r="I20" s="2">
-        <v>6</v>
-      </c>
+      <c r="I20" s="2"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D21">
         <v>110760</v>
@@ -856,9 +787,6 @@
         <v>110760</v>
       </c>
       <c r="H21">
-        <v>110760</v>
-      </c>
-      <c r="I21">
         <v>110760</v>
       </c>
     </row>
@@ -866,59 +794,53 @@
       <c r="B22" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="9">
         <f>10000/(D8/D21)</f>
         <v>2083.3333333333335</v>
       </c>
-      <c r="E22" s="18">
+      <c r="E22" s="9">
         <f>10000/(D8/D21)</f>
         <v>2083.3333333333335</v>
       </c>
-      <c r="F22" s="18">
+      <c r="F22" s="9">
         <f>10000/(D8/D21)</f>
         <v>2083.3333333333335</v>
       </c>
-      <c r="G22" s="18">
+      <c r="G22" s="9">
         <f>10000/(D8/D21)</f>
         <v>2083.3333333333335</v>
       </c>
-      <c r="H22" s="18">
+      <c r="H22" s="9">
         <f>10000/(D8/D21)</f>
         <v>2083.3333333333335</v>
       </c>
-      <c r="I22" s="18">
-        <f>10000/(D8/D21)</f>
-        <v>2083.3333333333335</v>
-      </c>
+      <c r="I22" s="9"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="18">
-        <f>25000/(531648/110760)</f>
+      <c r="D23" s="9">
+        <f t="shared" ref="D23:I23" si="0">25000/(531648/110760)</f>
         <v>5208.3333333333339</v>
       </c>
-      <c r="E23" s="18">
-        <f>25000/(531648/110760)</f>
+      <c r="E23" s="9">
+        <f t="shared" si="0"/>
         <v>5208.3333333333339</v>
       </c>
-      <c r="F23" s="18">
-        <f>25000/(531648/110760)</f>
+      <c r="F23" s="9">
+        <f t="shared" si="0"/>
         <v>5208.3333333333339</v>
       </c>
-      <c r="G23" s="18">
-        <f>25000/(531648/110760)</f>
+      <c r="G23" s="9">
+        <f t="shared" si="0"/>
         <v>5208.3333333333339</v>
       </c>
-      <c r="H23" s="18">
-        <f>25000/(531648/110760)</f>
+      <c r="H23" s="9">
+        <f t="shared" si="0"/>
         <v>5208.3333333333339</v>
       </c>
-      <c r="I23" s="18">
-        <f>25000/(531648/110760)</f>
-        <v>5208.3333333333339</v>
-      </c>
+      <c r="I23" s="9"/>
     </row>
     <row r="24" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
@@ -940,73 +862,64 @@
       <c r="H24" s="1">
         <v>-10526</v>
       </c>
-      <c r="I24" s="1">
-        <v>-10526</v>
-      </c>
+      <c r="I24" s="1"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>4</v>
       </c>
       <c r="D25">
-        <f>SUM(D21:D24)</f>
+        <f t="shared" ref="D25:I25" si="1">SUM(D21:D24)</f>
         <v>107525.66666666666</v>
       </c>
       <c r="E25">
-        <f>SUM(E21:E24)</f>
+        <f t="shared" si="1"/>
         <v>107525.66666666666</v>
       </c>
       <c r="F25">
-        <f>SUM(F21:F24)</f>
+        <f t="shared" si="1"/>
         <v>107525.66666666666</v>
       </c>
       <c r="G25">
-        <f>SUM(G21:G24)</f>
+        <f t="shared" si="1"/>
         <v>107525.66666666666</v>
       </c>
       <c r="H25">
-        <f>SUM(H21:H24)</f>
-        <v>107525.66666666666</v>
-      </c>
-      <c r="I25">
-        <f>SUM(I21:I24)</f>
+        <f t="shared" si="1"/>
         <v>107525.66666666666</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D26">
         <f>SUM(D25:I25)</f>
-        <v>645153.99999999988</v>
+        <v>537628.33333333326</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D27" s="5">
-        <f>(1+0.2143)^D20</f>
-        <v>1.2142999999999999</v>
+        <f>(1+0.26)^D20</f>
+        <v>1.26</v>
       </c>
       <c r="E27" s="5">
-        <f t="shared" ref="E27:I27" si="1">(1+0.2143)^E20</f>
-        <v>1.4745244899999999</v>
+        <f>(1+0.26)^E20</f>
+        <v>1.5876000000000001</v>
       </c>
       <c r="F27" s="5">
-        <f t="shared" si="1"/>
-        <v>1.7905150882069998</v>
+        <f>(1+0.26)^F20</f>
+        <v>2.0003760000000002</v>
       </c>
       <c r="G27" s="5">
-        <f t="shared" si="1"/>
-        <v>2.1742224716097596</v>
+        <f>(1+0.26)^G20</f>
+        <v>2.5204737600000002</v>
       </c>
       <c r="H27" s="5">
-        <f t="shared" si="1"/>
-        <v>2.6401583472757308</v>
-      </c>
-      <c r="I27" s="5">
-        <f t="shared" si="1"/>
-        <v>3.2059442810969201</v>
-      </c>
+        <f>(1+0.26)^H20</f>
+        <v>3.1757969376000004</v>
+      </c>
+      <c r="I27" s="5"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C28">
@@ -1015,47 +928,42 @@
       </c>
       <c r="D28">
         <f>D25/D27</f>
-        <v>88549.507260698883</v>
+        <v>85337.830687830676</v>
       </c>
       <c r="E28">
         <f t="shared" ref="E28:I28" si="2">E25/E27</f>
-        <v>72922.265717449467</v>
+        <v>67728.43705383387</v>
       </c>
       <c r="F28">
         <f t="shared" si="2"/>
-        <v>60052.924085851497</v>
+        <v>53752.727820503067</v>
       </c>
       <c r="G28">
         <f t="shared" si="2"/>
-        <v>49454.767426378574</v>
+        <v>42660.895095637359</v>
       </c>
       <c r="H28">
         <f t="shared" si="2"/>
-        <v>40726.976386707225</v>
-      </c>
-      <c r="I28">
-        <f t="shared" si="2"/>
-        <v>33539.468324719775</v>
+        <v>33857.853250505839</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D29">
         <f>C28+(SUM(D28:I28))</f>
-        <v>2591837.9092018055</v>
+        <v>2529929.7439083108</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="K4:M4"/>
-    <mergeCell ref="K6:M6"/>
     <mergeCell ref="K5:M5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D12 E12:G12 D25:I25" formulaRange="1"/>
+    <ignoredError sqref="D12:G12 D25:H25" formulaRange="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Apply more revisions to economic feasibility
</commit_message>
<xml_diff>
--- a/docs/flux.xlsx
+++ b/docs/flux.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BGM\Desktop\tesis\Thesis\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBEB917-7697-4BF8-9BAF-380ED5D7EAB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC786A63-3CC4-48D7-AC69-F660E1DEE2B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <author>BGM</author>
   </authors>
   <commentList>
-    <comment ref="C28" authorId="0" shapeId="0" xr:uid="{BD1A0333-F9E9-427D-AE3E-14E3FC7DF527}">
+    <comment ref="C26" authorId="0" shapeId="0" xr:uid="{BD1A0333-F9E9-427D-AE3E-14E3FC7DF527}">
       <text>
         <r>
           <rPr>
@@ -111,10 +111,10 @@
     <t>VAN</t>
   </si>
   <si>
-    <t>2. VAN (Mantenimiento del Proyecto)</t>
-  </si>
-  <si>
-    <t>2. VAN (Desarrollo del Proyecto)</t>
+    <t>2. Inversión Inicial</t>
+  </si>
+  <si>
+    <t>3. VAN (Mantenimiento del Proyecto)</t>
   </si>
 </sst>
 </file>
@@ -259,13 +259,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:N29"/>
+  <dimension ref="B2:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,7 +576,7 @@
       <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="10">
         <f>N4+N5+(N4*N5)</f>
         <v>0.26202999999999999</v>
       </c>
@@ -588,18 +588,18 @@
       <c r="N3" s="8"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="15">
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="11">
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
     <row r="5" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -608,12 +608,12 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="16">
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="12">
         <v>0.21</v>
       </c>
     </row>
@@ -736,224 +736,229 @@
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
     </row>
-    <row r="18" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="20" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="1"/>
-      <c r="C20" s="2">
+    <row r="16" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="18" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
+      <c r="C18" s="2">
         <v>0</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D18" s="2">
         <v>1</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E18" s="2">
         <v>2</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F18" s="2">
         <v>3</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G18" s="2">
         <v>4</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H18" s="2">
         <v>5</v>
       </c>
-      <c r="I20" s="2"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19">
+        <v>1329120</v>
+      </c>
+      <c r="E19">
+        <v>1329120</v>
+      </c>
+      <c r="F19">
+        <v>1329120</v>
+      </c>
+      <c r="G19">
+        <v>1329120</v>
+      </c>
+      <c r="H19">
+        <v>1329120</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="9">
+        <f>2083*12</f>
+        <v>24996</v>
+      </c>
+      <c r="E20" s="9">
+        <f t="shared" ref="E20:G20" si="0">2083*12</f>
+        <v>24996</v>
+      </c>
+      <c r="F20" s="9">
+        <f t="shared" si="0"/>
+        <v>24996</v>
+      </c>
+      <c r="G20" s="9">
+        <f t="shared" si="0"/>
+        <v>24996</v>
+      </c>
+      <c r="H20" s="9">
+        <f>2083*12</f>
+        <v>24996</v>
+      </c>
+      <c r="I20" s="9"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21">
-        <v>110760</v>
-      </c>
-      <c r="E21">
-        <v>110760</v>
-      </c>
-      <c r="F21">
-        <v>110760</v>
-      </c>
-      <c r="G21">
-        <v>110760</v>
-      </c>
-      <c r="H21">
-        <v>110760</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" s="9">
-        <f>10000/(D8/D21)</f>
-        <v>2083.3333333333335</v>
-      </c>
-      <c r="E22" s="9">
-        <f>10000/(D8/D21)</f>
-        <v>2083.3333333333335</v>
-      </c>
-      <c r="F22" s="9">
-        <f>10000/(D8/D21)</f>
-        <v>2083.3333333333335</v>
-      </c>
-      <c r="G22" s="9">
-        <f>10000/(D8/D21)</f>
-        <v>2083.3333333333335</v>
-      </c>
-      <c r="H22" s="9">
-        <f>10000/(D8/D21)</f>
-        <v>2083.3333333333335</v>
-      </c>
-      <c r="I22" s="9"/>
+        <v>2</v>
+      </c>
+      <c r="D21" s="9">
+        <f>5208*12</f>
+        <v>62496</v>
+      </c>
+      <c r="E21" s="9">
+        <f t="shared" ref="E21:G21" si="1">5208*12</f>
+        <v>62496</v>
+      </c>
+      <c r="F21" s="9">
+        <f t="shared" si="1"/>
+        <v>62496</v>
+      </c>
+      <c r="G21" s="9">
+        <f t="shared" si="1"/>
+        <v>62496</v>
+      </c>
+      <c r="H21" s="9">
+        <f>5208*12</f>
+        <v>62496</v>
+      </c>
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1">
+        <f>-10526*12</f>
+        <v>-126312</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" ref="E22:H22" si="2">-10526*12</f>
+        <v>-126312</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="2"/>
+        <v>-126312</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" si="2"/>
+        <v>-126312</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="2"/>
+        <v>-126312</v>
+      </c>
+      <c r="I22" s="1"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="9">
-        <f t="shared" ref="D23:I23" si="0">25000/(531648/110760)</f>
-        <v>5208.3333333333339</v>
-      </c>
-      <c r="E23" s="9">
-        <f t="shared" si="0"/>
-        <v>5208.3333333333339</v>
-      </c>
-      <c r="F23" s="9">
-        <f t="shared" si="0"/>
-        <v>5208.3333333333339</v>
-      </c>
-      <c r="G23" s="9">
-        <f t="shared" si="0"/>
-        <v>5208.3333333333339</v>
-      </c>
-      <c r="H23" s="9">
-        <f t="shared" si="0"/>
-        <v>5208.3333333333339</v>
-      </c>
-      <c r="I23" s="9"/>
-    </row>
-    <row r="24" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1">
-        <v>-10526</v>
-      </c>
-      <c r="E24" s="1">
-        <v>-10526</v>
-      </c>
-      <c r="F24" s="1">
-        <v>-10526</v>
-      </c>
-      <c r="G24" s="1">
-        <v>-10526</v>
-      </c>
-      <c r="H24" s="1">
-        <v>-10526</v>
-      </c>
-      <c r="I24" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ref="D23:H23" si="3">SUM(D19:D22)</f>
+        <v>1290300</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="3"/>
+        <v>1290300</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="3"/>
+        <v>1290300</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="3"/>
+        <v>1290300</v>
+      </c>
+      <c r="H23">
+        <f>SUM(H19:H22)</f>
+        <v>1290300</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24">
+        <f>SUM(D23:I23)</f>
+        <v>6451500</v>
+      </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25">
-        <f t="shared" ref="D25:I25" si="1">SUM(D21:D24)</f>
-        <v>107525.66666666666</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="1"/>
-        <v>107525.66666666666</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="1"/>
-        <v>107525.66666666666</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="1"/>
-        <v>107525.66666666666</v>
-      </c>
-      <c r="H25">
-        <f t="shared" si="1"/>
-        <v>107525.66666666666</v>
-      </c>
+      <c r="D25" s="5">
+        <f>(1+0.26)^D18</f>
+        <v>1.26</v>
+      </c>
+      <c r="E25" s="5">
+        <f>(1+0.26)^E18</f>
+        <v>1.5876000000000001</v>
+      </c>
+      <c r="F25" s="5">
+        <f>(1+0.26)^F18</f>
+        <v>2.0003760000000002</v>
+      </c>
+      <c r="G25" s="5">
+        <f>(1+0.26)^G18</f>
+        <v>2.5204737600000002</v>
+      </c>
+      <c r="H25" s="5">
+        <f>(1+0.26)^H18</f>
+        <v>3.1757969376000004</v>
+      </c>
+      <c r="I25" s="5"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26">
-        <f>SUM(D25:I25)</f>
-        <v>537628.33333333326</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D27" s="5">
-        <f>(1+0.26)^D20</f>
-        <v>1.26</v>
-      </c>
-      <c r="E27" s="5">
-        <f>(1+0.26)^E20</f>
-        <v>1.5876000000000001</v>
-      </c>
-      <c r="F27" s="5">
-        <f>(1+0.26)^F20</f>
-        <v>2.0003760000000002</v>
-      </c>
-      <c r="G27" s="5">
-        <f>(1+0.26)^G20</f>
-        <v>2.5204737600000002</v>
-      </c>
-      <c r="H27" s="5">
-        <f>(1+0.26)^H20</f>
-        <v>3.1757969376000004</v>
-      </c>
-      <c r="I27" s="5"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C28">
+      <c r="C26">
         <f>D13</f>
         <v>2246592</v>
       </c>
-      <c r="D28">
-        <f>D25/D27</f>
-        <v>85337.830687830676</v>
-      </c>
-      <c r="E28">
-        <f t="shared" ref="E28:I28" si="2">E25/E27</f>
-        <v>67728.43705383387</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="2"/>
-        <v>53752.727820503067</v>
-      </c>
-      <c r="G28">
-        <f t="shared" si="2"/>
-        <v>42660.895095637359</v>
-      </c>
-      <c r="H28">
-        <f t="shared" si="2"/>
-        <v>33857.853250505839</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+      <c r="D26">
+        <f>D23/D25</f>
+        <v>1024047.6190476191</v>
+      </c>
+      <c r="E26">
+        <f t="shared" ref="E26:H26" si="4">E23/E25</f>
+        <v>812736.20559334836</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="4"/>
+        <v>645028.73459789553</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="4"/>
+        <v>511927.56714118691</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="4"/>
+        <v>406291.71995332296</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>12</v>
       </c>
-      <c r="D29">
-        <f>C28+(SUM(D28:I28))</f>
-        <v>2529929.7439083108</v>
+      <c r="D27">
+        <f>C26+(SUM(D26:I26))</f>
+        <v>5646623.8463333733</v>
       </c>
     </row>
   </sheetData>
@@ -963,7 +968,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D12:G12 D25:H25" formulaRange="1"/>
+    <ignoredError sqref="D12:G12" formulaRange="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>